<commit_message>
Before updating BBU function after reviews
</commit_message>
<xml_diff>
--- a/tabelas/energy-table.xlsx
+++ b/tabelas/energy-table.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">FH (fixo)</t>
   </si>
   <si>
-    <t xml:space="preserve">BBU daEdge</t>
+    <t xml:space="preserve">BBU Edge</t>
   </si>
   <si>
     <t xml:space="preserve">BBU Cloud</t>
@@ -144,7 +144,7 @@
   <dimension ref="B1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>